<commit_message>
new data 2.2.21 (from 31.1.21)
</commit_message>
<xml_diff>
--- a/impf_daten.xlsx
+++ b/impf_daten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DC82DF-3B33-4B13-97E8-77D78FAEEBE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2A2DAE-358F-44E8-AB08-BCF00B64E48B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="87">
   <si>
     <t>Kanton</t>
   </si>
@@ -363,13 +363,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -709,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O128"/>
+  <dimension ref="A1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6733,6 +6734,448 @@
       </c>
       <c r="O128">
         <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" t="s">
+        <v>47</v>
+      </c>
+      <c r="D129">
+        <v>18012</v>
+      </c>
+      <c r="H129">
+        <v>3.57</v>
+      </c>
+      <c r="J129" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>36</v>
+      </c>
+      <c r="C130" t="s">
+        <v>62</v>
+      </c>
+      <c r="D130">
+        <v>27848</v>
+      </c>
+      <c r="H130">
+        <v>3.46</v>
+      </c>
+      <c r="J130" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" t="s">
+        <v>63</v>
+      </c>
+      <c r="D131">
+        <v>14240</v>
+      </c>
+      <c r="H131">
+        <v>4.12</v>
+      </c>
+      <c r="J131" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" t="s">
+        <v>46</v>
+      </c>
+      <c r="D132">
+        <v>9580</v>
+      </c>
+      <c r="H132">
+        <v>2.98</v>
+      </c>
+      <c r="J132" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>26</v>
+      </c>
+      <c r="C133" t="s">
+        <v>52</v>
+      </c>
+      <c r="D133">
+        <v>4907</v>
+      </c>
+      <c r="H133">
+        <v>2.78</v>
+      </c>
+      <c r="J133" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>24</v>
+      </c>
+      <c r="C134" t="s">
+        <v>50</v>
+      </c>
+      <c r="D134">
+        <v>2792</v>
+      </c>
+      <c r="H134">
+        <v>3.79</v>
+      </c>
+      <c r="J134" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>17</v>
+      </c>
+      <c r="C135" t="s">
+        <v>43</v>
+      </c>
+      <c r="D135">
+        <v>24385</v>
+      </c>
+      <c r="H135">
+        <v>2.35</v>
+      </c>
+      <c r="J135" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>31</v>
+      </c>
+      <c r="C136" t="s">
+        <v>57</v>
+      </c>
+      <c r="D136">
+        <v>15099</v>
+      </c>
+      <c r="H136">
+        <v>5.49</v>
+      </c>
+      <c r="J136" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="137" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" t="s">
+        <v>45</v>
+      </c>
+      <c r="D137">
+        <v>13754</v>
+      </c>
+      <c r="H137">
+        <v>7.02</v>
+      </c>
+      <c r="J137" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>18</v>
+      </c>
+      <c r="C138" t="s">
+        <v>44</v>
+      </c>
+      <c r="D138">
+        <v>11364</v>
+      </c>
+      <c r="H138">
+        <v>3.93</v>
+      </c>
+      <c r="J138" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>14</v>
+      </c>
+      <c r="C139" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139">
+        <v>20034</v>
+      </c>
+      <c r="H139">
+        <v>2.92</v>
+      </c>
+      <c r="J139" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>39</v>
+      </c>
+      <c r="C140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140">
+        <v>46081</v>
+      </c>
+      <c r="H140">
+        <v>2.99</v>
+      </c>
+      <c r="J140" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>30</v>
+      </c>
+      <c r="C141" t="s">
+        <v>56</v>
+      </c>
+      <c r="D141">
+        <v>5685</v>
+      </c>
+      <c r="H141">
+        <v>6.9</v>
+      </c>
+      <c r="J141" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" t="s">
+        <v>59</v>
+      </c>
+      <c r="D142">
+        <v>8868</v>
+      </c>
+      <c r="H142">
+        <v>3.17</v>
+      </c>
+      <c r="J142" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="143" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+      <c r="C143" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143">
+        <v>3542</v>
+      </c>
+      <c r="H143">
+        <v>6.39</v>
+      </c>
+      <c r="J143" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="144" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" t="s">
+        <v>41</v>
+      </c>
+      <c r="D144">
+        <v>1092</v>
+      </c>
+      <c r="H144">
+        <v>6.77</v>
+      </c>
+      <c r="J144" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>29</v>
+      </c>
+      <c r="C145" t="s">
+        <v>55</v>
+      </c>
+      <c r="D145">
+        <v>19281</v>
+      </c>
+      <c r="H145">
+        <v>3.78</v>
+      </c>
+      <c r="J145" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>22</v>
+      </c>
+      <c r="C146" t="s">
+        <v>48</v>
+      </c>
+      <c r="D146">
+        <v>2330</v>
+      </c>
+      <c r="H146">
+        <v>5.74</v>
+      </c>
+      <c r="J146" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>32</v>
+      </c>
+      <c r="C147" t="s">
+        <v>58</v>
+      </c>
+      <c r="D147">
+        <v>5165</v>
+      </c>
+      <c r="H147">
+        <v>3.22</v>
+      </c>
+      <c r="J147" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>38</v>
+      </c>
+      <c r="C148" t="s">
+        <v>64</v>
+      </c>
+      <c r="D148">
+        <v>7431</v>
+      </c>
+      <c r="H148">
+        <v>5.82</v>
+      </c>
+      <c r="J148" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" t="s">
+        <v>51</v>
+      </c>
+      <c r="D149">
+        <v>18076</v>
+      </c>
+      <c r="H149">
+        <v>4.38</v>
+      </c>
+      <c r="J149" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>27</v>
+      </c>
+      <c r="C150" t="s">
+        <v>53</v>
+      </c>
+      <c r="D150">
+        <v>3218</v>
+      </c>
+      <c r="H150">
+        <v>7.47</v>
+      </c>
+      <c r="J150" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>28</v>
+      </c>
+      <c r="C151" t="s">
+        <v>54</v>
+      </c>
+      <c r="D151">
+        <v>2156</v>
+      </c>
+      <c r="H151">
+        <v>5.68</v>
+      </c>
+      <c r="J151" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>35</v>
+      </c>
+      <c r="C152" t="s">
+        <v>61</v>
+      </c>
+      <c r="D152">
+        <v>2184</v>
+      </c>
+      <c r="H152">
+        <v>5.95</v>
+      </c>
+      <c r="J152" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>23</v>
+      </c>
+      <c r="C153" t="s">
+        <v>49</v>
+      </c>
+      <c r="D153">
+        <v>7339</v>
+      </c>
+      <c r="H153">
+        <v>3.69</v>
+      </c>
+      <c r="J153" s="4">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>34</v>
+      </c>
+      <c r="C154" t="s">
+        <v>60</v>
+      </c>
+      <c r="D154">
+        <v>19737</v>
+      </c>
+      <c r="H154">
+        <v>5.62</v>
+      </c>
+      <c r="J154" s="4">
+        <v>44227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>